<commit_message>
uploaded correlation coefficient results
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Monash_University\Year5\Honours_Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065BB330-2BE1-4CAB-AC81-6F85BDA9335B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F29BA5-EB58-4D20-B099-918B791B335F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{52DF0958-0AB4-4740-8193-FA00E6A62DB5}"/>
+    <workbookView xWindow="-28920" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{52DF0958-0AB4-4740-8193-FA00E6A62DB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Old" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="66">
   <si>
     <t>TSN = Total number of generated samples</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>native_country</t>
+  </si>
+  <si>
+    <t>Feature</t>
   </si>
 </sst>
 </file>
@@ -3753,9 +3756,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42F29A4-40B4-4F76-862E-2F3EC1AC93BE}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3801,30 +3804,30 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:25">
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="73" t="s">
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="73" t="s">
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="73" t="s">
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="75"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="78"/>
       <c r="R4" s="76" t="s">
         <v>18</v>
       </c>
@@ -4204,30 +4207,30 @@
       <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:25">
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="73" t="s">
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="73" t="s">
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="74"/>
-      <c r="L12" s="74"/>
-      <c r="M12" s="75"/>
-      <c r="N12" s="73" t="s">
+      <c r="K12" s="77"/>
+      <c r="L12" s="77"/>
+      <c r="M12" s="78"/>
+      <c r="N12" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="O12" s="74"/>
-      <c r="P12" s="74"/>
-      <c r="Q12" s="75"/>
+      <c r="O12" s="77"/>
+      <c r="P12" s="77"/>
+      <c r="Q12" s="78"/>
       <c r="R12" s="76" t="s">
         <v>18</v>
       </c>
@@ -4608,30 +4611,30 @@
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:25">
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="73" t="s">
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="74"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="75"/>
-      <c r="J20" s="73" t="s">
+      <c r="G20" s="77"/>
+      <c r="H20" s="77"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="75"/>
-      <c r="N20" s="73" t="s">
+      <c r="K20" s="77"/>
+      <c r="L20" s="77"/>
+      <c r="M20" s="78"/>
+      <c r="N20" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="O20" s="74"/>
-      <c r="P20" s="74"/>
-      <c r="Q20" s="75"/>
+      <c r="O20" s="77"/>
+      <c r="P20" s="77"/>
+      <c r="Q20" s="78"/>
       <c r="R20" s="76" t="s">
         <v>18</v>
       </c>
@@ -5017,8 +5020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8137F2D2-9415-4E0A-902C-EE90A5695E2E}">
   <dimension ref="A3:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5037,6 +5040,9 @@
       </c>
     </row>
     <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
       <c r="B5" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
calculated p-values, t-test and graphs
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Monash_University\Year5\Honours_Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F29BA5-EB58-4D20-B099-918B791B335F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBE1BA8-A0E1-44A1-AFE9-7FE77D8AD098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{52DF0958-0AB4-4740-8193-FA00E6A62DB5}"/>
+    <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{52DF0958-0AB4-4740-8193-FA00E6A62DB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Old" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="general data" sheetId="5" r:id="rId3"/>
     <sheet name="new_data" sheetId="6" r:id="rId4"/>
     <sheet name="correlation_coefficients" sheetId="8" r:id="rId5"/>
+    <sheet name="t-test" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="73">
   <si>
     <t>TSN = Total number of generated samples</t>
   </si>
@@ -238,6 +239,27 @@
   </si>
   <si>
     <t>Feature</t>
+  </si>
+  <si>
+    <t>Fairness Testing Algorithm</t>
+  </si>
+  <si>
+    <t>Classifier</t>
+  </si>
+  <si>
+    <t>t-statistic</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>Reject Null Hypothesis</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Reject null hypthesis?</t>
   </si>
 </sst>
 </file>
@@ -434,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -528,6 +550,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3756,9 +3779,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42F29A4-40B4-4F76-862E-2F3EC1AC93BE}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N9" sqref="N9"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4878,17 +4901,17 @@
         <v>0.69201042483677699</v>
       </c>
       <c r="V23" s="65">
-        <v>58399.72</v>
+        <v>68850.64</v>
       </c>
       <c r="W23" s="66">
-        <v>37408.92</v>
+        <v>47900.56</v>
       </c>
       <c r="X23" s="67">
-        <v>30.305739288329999</v>
+        <v>29.520818271636902</v>
       </c>
       <c r="Y23" s="68">
-        <f>0.64057186374492</f>
-        <v>0.64057186374492003</v>
+        <f>0.695717701367691</f>
+        <v>0.69571770136769095</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -4976,19 +4999,19 @@
       </c>
       <c r="V25" s="2">
         <f>V23-R23</f>
-        <v>-13751.559999999998</v>
+        <v>-3300.6399999999994</v>
       </c>
       <c r="W25" s="2">
         <f t="shared" ref="W25:Y25" si="9">W23-S23</f>
-        <v>-12520.279999999999</v>
+        <v>-2028.6399999999994</v>
       </c>
       <c r="X25" s="60">
-        <f t="shared" si="9"/>
-        <v>-2.1975547409058045</v>
+        <f>X23-T23</f>
+        <v>-2.9824757575989018</v>
       </c>
       <c r="Y25" s="70">
         <f t="shared" si="9"/>
-        <v>-5.143856109185696E-2</v>
+        <v>3.707276530913961E-3</v>
       </c>
     </row>
   </sheetData>
@@ -6044,4 +6067,766 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95DB78E-C3C9-4D84-AB69-47409FDD14D6}">
+  <dimension ref="B3:G42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7">
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4">
+        <v>-1.1693913956591699</v>
+      </c>
+      <c r="F4">
+        <v>0.25372924677457598</v>
+      </c>
+      <c r="G4" t="b">
+        <f>F4&lt;0.05</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5">
+        <v>-0.31776652576627101</v>
+      </c>
+      <c r="F5">
+        <v>0.75341035855965799</v>
+      </c>
+      <c r="G5" t="b">
+        <f t="shared" ref="G5:G21" si="0">F5&lt;0.05</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6">
+        <v>-23.426223312313699</v>
+      </c>
+      <c r="F6" s="79">
+        <v>4.8137919979846798E-18</v>
+      </c>
+      <c r="G6" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7">
+        <v>-14.297332990836001</v>
+      </c>
+      <c r="F7" s="79">
+        <v>3.0714612725714102E-13</v>
+      </c>
+      <c r="G7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8">
+        <v>-0.41377015356941399</v>
+      </c>
+      <c r="F8">
+        <v>0.68271670620649105</v>
+      </c>
+      <c r="G8" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9">
+        <v>-4.0814472340827601</v>
+      </c>
+      <c r="F9">
+        <v>4.2880921906591899E-4</v>
+      </c>
+      <c r="G9" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10">
+        <v>-12.112149888197999</v>
+      </c>
+      <c r="F10" s="79">
+        <v>1.03067926866572E-11</v>
+      </c>
+      <c r="G10" t="b">
+        <f>F10&lt;0.05</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11">
+        <v>-0.46110818639969398</v>
+      </c>
+      <c r="F11">
+        <v>0.64887258439009499</v>
+      </c>
+      <c r="G11" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12">
+        <v>1.06041085590896</v>
+      </c>
+      <c r="F12">
+        <v>0.29951326413134899</v>
+      </c>
+      <c r="G12" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13">
+        <v>-2.9256685367686099</v>
+      </c>
+      <c r="F13">
+        <v>7.3993424288121296E-3</v>
+      </c>
+      <c r="G13" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14">
+        <v>-6.8462529407336197</v>
+      </c>
+      <c r="F14" s="79">
+        <v>4.4238056566889001E-7</v>
+      </c>
+      <c r="G14" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15">
+        <v>0.70881419932388401</v>
+      </c>
+      <c r="F15">
+        <v>0.48526860203996602</v>
+      </c>
+      <c r="G15" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16">
+        <v>-30.993361936174601</v>
+      </c>
+      <c r="F16" s="79">
+        <v>7.1735146545689301E-21</v>
+      </c>
+      <c r="G16" t="b">
+        <f>F16&lt;0.05</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17">
+        <v>-0.42922691283650499</v>
+      </c>
+      <c r="F17">
+        <v>0.67158672847322398</v>
+      </c>
+      <c r="G17" t="b">
+        <f>F17&lt;0.05</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18">
+        <v>-23.426223312313699</v>
+      </c>
+      <c r="F18" s="79">
+        <v>4.8137919979846798E-18</v>
+      </c>
+      <c r="G18" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19">
+        <v>0.349556455790973</v>
+      </c>
+      <c r="F19">
+        <v>0.72972028676733203</v>
+      </c>
+      <c r="G19" t="b">
+        <f>F19&lt;0.05</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20">
+        <v>-2.2221621609410001</v>
+      </c>
+      <c r="F20">
+        <v>3.5952710792857202E-2</v>
+      </c>
+      <c r="G20" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21">
+        <v>-96.983270019834706</v>
+      </c>
+      <c r="F21" s="79">
+        <v>1.1922100634926601E-32</v>
+      </c>
+      <c r="G21" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25">
+        <v>0.25372924677457598</v>
+      </c>
+      <c r="F25" s="1" t="str">
+        <f>IF(E25&lt;0.05, "Yes", "No")</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26">
+        <v>0.75341035855965799</v>
+      </c>
+      <c r="F26" s="1" t="str">
+        <f t="shared" ref="F26:F42" si="1">IF(E26&lt;0.05, "Yes", "No")</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="79">
+        <v>4.8137919979846798E-18</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="79">
+        <v>3.0714612725714102E-13</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29">
+        <v>0.68271670620649105</v>
+      </c>
+      <c r="F29" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30">
+        <v>4.2880921906591899E-4</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="79">
+        <v>1.03067926866572E-11</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32">
+        <v>0.64887258439009499</v>
+      </c>
+      <c r="F32" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33">
+        <v>0.29951326413134899</v>
+      </c>
+      <c r="F33" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34">
+        <v>7.3993424288121296E-3</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" s="79">
+        <v>4.4238056566889001E-7</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36">
+        <v>0.48526860203996602</v>
+      </c>
+      <c r="F36" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" s="79">
+        <v>7.1735146545689301E-21</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38">
+        <v>0.67158672847322398</v>
+      </c>
+      <c r="F38" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="79">
+        <v>4.8137919979846798E-18</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40">
+        <v>0.72972028676733203</v>
+      </c>
+      <c r="F40" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41">
+        <v>3.5952710792857202E-2</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="79">
+        <v>1.1922100634926601E-32</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added calc for time paired t test
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Monash_University\Year5\Honours_Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456E31BE-2683-47DF-B829-DF499C01F8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7897E318-15D4-46F1-BF46-D6CA28AA1C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{52DF0958-0AB4-4740-8193-FA00E6A62DB5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{52DF0958-0AB4-4740-8193-FA00E6A62DB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Old" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="t-test" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="79">
   <si>
     <t>TSN = Total number of generated samples</t>
   </si>
@@ -257,13 +258,28 @@
     <t>Reject Null Hypothesis</t>
   </si>
   <si>
-    <t>P-value</t>
+    <t>Time</t>
   </si>
   <si>
-    <t>Reject null hypthesis?</t>
+    <t>SUR P-value</t>
   </si>
   <si>
-    <t>Time</t>
+    <t>Time P-Value</t>
+  </si>
+  <si>
+    <t>Reject Time Null</t>
+  </si>
+  <si>
+    <t>Reject SUR Null</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Combined Results</t>
   </si>
 </sst>
 </file>
@@ -460,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -536,6 +552,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -554,14 +574,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -947,30 +962,30 @@
       </c>
     </row>
     <row r="14" spans="2:19">
-      <c r="D14" s="73" t="s">
+      <c r="D14" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="73" t="s">
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="74"/>
-      <c r="J14" s="74"/>
-      <c r="K14" s="75"/>
-      <c r="L14" s="73" t="s">
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="74"/>
-      <c r="N14" s="74"/>
-      <c r="O14" s="75"/>
-      <c r="P14" s="73" t="s">
+      <c r="M14" s="78"/>
+      <c r="N14" s="78"/>
+      <c r="O14" s="79"/>
+      <c r="P14" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="Q14" s="74"/>
-      <c r="R14" s="74"/>
-      <c r="S14" s="75"/>
+      <c r="Q14" s="78"/>
+      <c r="R14" s="78"/>
+      <c r="S14" s="79"/>
     </row>
     <row r="15" spans="2:19">
       <c r="D15" s="5" t="s">
@@ -1128,30 +1143,30 @@
       </c>
     </row>
     <row r="22" spans="3:19">
-      <c r="D22" s="73" t="s">
+      <c r="D22" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="73" t="s">
+      <c r="E22" s="78"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="75"/>
-      <c r="L22" s="73" t="s">
+      <c r="I22" s="78"/>
+      <c r="J22" s="78"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="M22" s="74"/>
-      <c r="N22" s="74"/>
-      <c r="O22" s="75"/>
-      <c r="P22" s="73" t="s">
+      <c r="M22" s="78"/>
+      <c r="N22" s="78"/>
+      <c r="O22" s="79"/>
+      <c r="P22" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="Q22" s="74"/>
-      <c r="R22" s="74"/>
-      <c r="S22" s="75"/>
+      <c r="Q22" s="78"/>
+      <c r="R22" s="78"/>
+      <c r="S22" s="79"/>
     </row>
     <row r="23" spans="3:19">
       <c r="D23" s="5" t="s">
@@ -1300,30 +1315,30 @@
       </c>
     </row>
     <row r="30" spans="3:19">
-      <c r="D30" s="73" t="s">
+      <c r="D30" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="73" t="s">
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="I30" s="74"/>
-      <c r="J30" s="74"/>
-      <c r="K30" s="75"/>
-      <c r="L30" s="73" t="s">
+      <c r="I30" s="78"/>
+      <c r="J30" s="78"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="M30" s="74"/>
-      <c r="N30" s="74"/>
-      <c r="O30" s="75"/>
-      <c r="P30" s="73" t="s">
+      <c r="M30" s="78"/>
+      <c r="N30" s="78"/>
+      <c r="O30" s="79"/>
+      <c r="P30" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="Q30" s="74"/>
-      <c r="R30" s="74"/>
-      <c r="S30" s="75"/>
+      <c r="Q30" s="78"/>
+      <c r="R30" s="78"/>
+      <c r="S30" s="79"/>
     </row>
     <row r="31" spans="3:19">
       <c r="D31" s="5" t="s">
@@ -1543,42 +1558,42 @@
       <c r="R3" s="14"/>
     </row>
     <row r="4" spans="2:26">
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="73" t="s">
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="73" t="s">
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="74"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="75"/>
-      <c r="O4" s="73" t="s">
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="75"/>
-      <c r="S4" s="73" t="s">
+      <c r="P4" s="78"/>
+      <c r="Q4" s="78"/>
+      <c r="R4" s="79"/>
+      <c r="S4" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="T4" s="74"/>
-      <c r="U4" s="74"/>
-      <c r="V4" s="75"/>
-      <c r="W4" s="73" t="s">
+      <c r="T4" s="78"/>
+      <c r="U4" s="78"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="X4" s="74"/>
-      <c r="Y4" s="74"/>
-      <c r="Z4" s="75"/>
+      <c r="X4" s="78"/>
+      <c r="Y4" s="78"/>
+      <c r="Z4" s="79"/>
     </row>
     <row r="5" spans="2:26">
       <c r="B5" s="33" t="s">
@@ -1869,42 +1884,42 @@
       <c r="R11" s="14"/>
     </row>
     <row r="12" spans="2:26">
-      <c r="C12" s="73" t="s">
+      <c r="C12" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="73" t="s">
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="73" t="s">
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="L12" s="74"/>
-      <c r="M12" s="74"/>
-      <c r="N12" s="75"/>
-      <c r="O12" s="73" t="s">
+      <c r="L12" s="78"/>
+      <c r="M12" s="78"/>
+      <c r="N12" s="79"/>
+      <c r="O12" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="P12" s="74"/>
-      <c r="Q12" s="74"/>
-      <c r="R12" s="75"/>
-      <c r="S12" s="73" t="s">
+      <c r="P12" s="78"/>
+      <c r="Q12" s="78"/>
+      <c r="R12" s="79"/>
+      <c r="S12" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="T12" s="74"/>
-      <c r="U12" s="74"/>
-      <c r="V12" s="75"/>
-      <c r="W12" s="73" t="s">
+      <c r="T12" s="78"/>
+      <c r="U12" s="78"/>
+      <c r="V12" s="79"/>
+      <c r="W12" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="X12" s="74"/>
-      <c r="Y12" s="74"/>
-      <c r="Z12" s="75"/>
+      <c r="X12" s="78"/>
+      <c r="Y12" s="78"/>
+      <c r="Z12" s="79"/>
     </row>
     <row r="13" spans="2:26">
       <c r="B13" s="33" t="s">
@@ -2196,42 +2211,42 @@
       <c r="R19" s="14"/>
     </row>
     <row r="20" spans="2:26">
-      <c r="C20" s="73" t="s">
+      <c r="C20" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="73" t="s">
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="75"/>
-      <c r="K20" s="73" t="s">
+      <c r="H20" s="78"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="79"/>
+      <c r="K20" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="L20" s="74"/>
-      <c r="M20" s="74"/>
-      <c r="N20" s="75"/>
-      <c r="O20" s="73" t="s">
+      <c r="L20" s="78"/>
+      <c r="M20" s="78"/>
+      <c r="N20" s="79"/>
+      <c r="O20" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="P20" s="74"/>
-      <c r="Q20" s="74"/>
-      <c r="R20" s="75"/>
-      <c r="S20" s="73" t="s">
+      <c r="P20" s="78"/>
+      <c r="Q20" s="78"/>
+      <c r="R20" s="79"/>
+      <c r="S20" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="T20" s="74"/>
-      <c r="U20" s="74"/>
-      <c r="V20" s="75"/>
-      <c r="W20" s="73" t="s">
+      <c r="T20" s="78"/>
+      <c r="U20" s="78"/>
+      <c r="V20" s="79"/>
+      <c r="W20" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="X20" s="74"/>
-      <c r="Y20" s="74"/>
-      <c r="Z20" s="75"/>
+      <c r="X20" s="78"/>
+      <c r="Y20" s="78"/>
+      <c r="Z20" s="79"/>
     </row>
     <row r="21" spans="2:26">
       <c r="B21" s="33" t="s">
@@ -2492,11 +2507,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="W4:Z4"/>
-    <mergeCell ref="S12:V12"/>
-    <mergeCell ref="W12:Z12"/>
-    <mergeCell ref="S20:V20"/>
-    <mergeCell ref="W20:Z20"/>
     <mergeCell ref="C20:F20"/>
     <mergeCell ref="G20:J20"/>
     <mergeCell ref="K20:N20"/>
@@ -2510,6 +2520,11 @@
     <mergeCell ref="G12:J12"/>
     <mergeCell ref="K12:N12"/>
     <mergeCell ref="O12:R12"/>
+    <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="S12:V12"/>
+    <mergeCell ref="W12:Z12"/>
+    <mergeCell ref="S20:V20"/>
+    <mergeCell ref="W20:Z20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2563,42 +2578,42 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:25">
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="73" t="s">
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="73" t="s">
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="73" t="s">
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="79"/>
+      <c r="N4" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="75"/>
-      <c r="R4" s="76" t="s">
+      <c r="O4" s="78"/>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="77"/>
-      <c r="T4" s="77"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="76" t="s">
+      <c r="S4" s="81"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="82"/>
+      <c r="V4" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="W4" s="77"/>
-      <c r="X4" s="77"/>
-      <c r="Y4" s="78"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="33" t="s">
@@ -2970,42 +2985,42 @@
       <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:25">
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="73" t="s">
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="73" t="s">
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="74"/>
-      <c r="L12" s="74"/>
-      <c r="M12" s="75"/>
-      <c r="N12" s="73" t="s">
+      <c r="K12" s="78"/>
+      <c r="L12" s="78"/>
+      <c r="M12" s="79"/>
+      <c r="N12" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="O12" s="74"/>
-      <c r="P12" s="74"/>
-      <c r="Q12" s="75"/>
-      <c r="R12" s="76" t="s">
+      <c r="O12" s="78"/>
+      <c r="P12" s="78"/>
+      <c r="Q12" s="79"/>
+      <c r="R12" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="S12" s="77"/>
-      <c r="T12" s="77"/>
-      <c r="U12" s="78"/>
-      <c r="V12" s="76" t="s">
+      <c r="S12" s="81"/>
+      <c r="T12" s="81"/>
+      <c r="U12" s="82"/>
+      <c r="V12" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="W12" s="77"/>
-      <c r="X12" s="77"/>
-      <c r="Y12" s="78"/>
+      <c r="W12" s="81"/>
+      <c r="X12" s="81"/>
+      <c r="Y12" s="82"/>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="33" t="s">
@@ -3378,42 +3393,42 @@
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:25">
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="73" t="s">
+      <c r="C20" s="78"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="74"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="75"/>
-      <c r="J20" s="73" t="s">
+      <c r="G20" s="78"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="75"/>
-      <c r="N20" s="73" t="s">
+      <c r="K20" s="78"/>
+      <c r="L20" s="78"/>
+      <c r="M20" s="79"/>
+      <c r="N20" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="O20" s="74"/>
-      <c r="P20" s="74"/>
-      <c r="Q20" s="75"/>
-      <c r="R20" s="76" t="s">
+      <c r="O20" s="78"/>
+      <c r="P20" s="78"/>
+      <c r="Q20" s="79"/>
+      <c r="R20" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="S20" s="77"/>
-      <c r="T20" s="77"/>
-      <c r="U20" s="78"/>
-      <c r="V20" s="76" t="s">
+      <c r="S20" s="81"/>
+      <c r="T20" s="81"/>
+      <c r="U20" s="82"/>
+      <c r="V20" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="W20" s="77"/>
-      <c r="X20" s="77"/>
-      <c r="Y20" s="78"/>
+      <c r="W20" s="81"/>
+      <c r="X20" s="81"/>
+      <c r="Y20" s="82"/>
     </row>
     <row r="21" spans="1:25">
       <c r="A21" s="33" t="s">
@@ -3763,12 +3778,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="V4:Y4"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:U4"/>
     <mergeCell ref="V20:Y20"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="F12:I12"/>
@@ -3781,6 +3790,12 @@
     <mergeCell ref="J20:M20"/>
     <mergeCell ref="N20:Q20"/>
     <mergeCell ref="R20:U20"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:U4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3838,42 +3853,42 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:25">
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="76" t="s">
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="76" t="s">
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="77"/>
-      <c r="L4" s="77"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="76" t="s">
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="77"/>
-      <c r="P4" s="77"/>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="76" t="s">
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="82"/>
+      <c r="R4" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="77"/>
-      <c r="T4" s="77"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="76" t="s">
+      <c r="S4" s="81"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="82"/>
+      <c r="V4" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="W4" s="77"/>
-      <c r="X4" s="77"/>
-      <c r="Y4" s="78"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="33" t="s">
@@ -4241,42 +4256,42 @@
       <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:25">
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="76" t="s">
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="76" t="s">
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="77"/>
-      <c r="L12" s="77"/>
-      <c r="M12" s="78"/>
-      <c r="N12" s="76" t="s">
+      <c r="K12" s="81"/>
+      <c r="L12" s="81"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="O12" s="77"/>
-      <c r="P12" s="77"/>
-      <c r="Q12" s="78"/>
-      <c r="R12" s="76" t="s">
+      <c r="O12" s="81"/>
+      <c r="P12" s="81"/>
+      <c r="Q12" s="82"/>
+      <c r="R12" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="S12" s="77"/>
-      <c r="T12" s="77"/>
-      <c r="U12" s="78"/>
-      <c r="V12" s="76" t="s">
+      <c r="S12" s="81"/>
+      <c r="T12" s="81"/>
+      <c r="U12" s="82"/>
+      <c r="V12" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="W12" s="77"/>
-      <c r="X12" s="77"/>
-      <c r="Y12" s="78"/>
+      <c r="W12" s="81"/>
+      <c r="X12" s="81"/>
+      <c r="Y12" s="82"/>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="33" t="s">
@@ -4645,42 +4660,42 @@
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:25">
-      <c r="B20" s="76" t="s">
+      <c r="B20" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="77"/>
-      <c r="D20" s="77"/>
-      <c r="E20" s="78"/>
-      <c r="F20" s="76" t="s">
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="77"/>
-      <c r="H20" s="77"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="76" t="s">
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="77"/>
-      <c r="L20" s="77"/>
-      <c r="M20" s="78"/>
-      <c r="N20" s="76" t="s">
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="82"/>
+      <c r="N20" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="O20" s="77"/>
-      <c r="P20" s="77"/>
-      <c r="Q20" s="78"/>
-      <c r="R20" s="76" t="s">
+      <c r="O20" s="81"/>
+      <c r="P20" s="81"/>
+      <c r="Q20" s="82"/>
+      <c r="R20" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="S20" s="77"/>
-      <c r="T20" s="77"/>
-      <c r="U20" s="78"/>
-      <c r="V20" s="76" t="s">
+      <c r="S20" s="81"/>
+      <c r="T20" s="81"/>
+      <c r="U20" s="82"/>
+      <c r="V20" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="W20" s="77"/>
-      <c r="X20" s="77"/>
-      <c r="Y20" s="78"/>
+      <c r="W20" s="81"/>
+      <c r="X20" s="81"/>
+      <c r="Y20" s="82"/>
     </row>
     <row r="21" spans="1:25">
       <c r="A21" s="33" t="s">
@@ -5027,6 +5042,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:U4"/>
     <mergeCell ref="V20:Y20"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="F12:I12"/>
@@ -5039,12 +5060,6 @@
     <mergeCell ref="J20:M20"/>
     <mergeCell ref="N20:Q20"/>
     <mergeCell ref="R20:U20"/>
-    <mergeCell ref="V4:Y4"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:U4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5054,7 +5069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9DC7D24-B396-4993-B282-4FF11F71EEA8}">
   <dimension ref="A2:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="V10" sqref="V10"/>
     </sheetView>
@@ -5088,7 +5103,7 @@
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="80"/>
+      <c r="D2" s="74"/>
       <c r="F2" s="14"/>
       <c r="L2" t="s">
         <v>22</v>
@@ -5104,48 +5119,48 @@
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:31">
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="76" t="s">
+      <c r="C4" s="81"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="77"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="76" t="s">
+      <c r="H4" s="81"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="77"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="77"/>
-      <c r="P4" s="78"/>
-      <c r="Q4" s="76" t="s">
+      <c r="M4" s="81"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="77"/>
-      <c r="S4" s="81"/>
-      <c r="T4" s="77"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="76" t="s">
+      <c r="R4" s="81"/>
+      <c r="S4" s="83"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="82"/>
+      <c r="V4" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="W4" s="77"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="77"/>
-      <c r="Z4" s="78"/>
-      <c r="AA4" s="76" t="s">
+      <c r="W4" s="81"/>
+      <c r="X4" s="83"/>
+      <c r="Y4" s="81"/>
+      <c r="Z4" s="82"/>
+      <c r="AA4" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="AB4" s="77"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="77"/>
-      <c r="AE4" s="78"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="83"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="82"/>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" s="33" t="s">
@@ -5161,7 +5176,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>8</v>
@@ -5176,7 +5191,7 @@
         <v>7</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K5" s="15" t="s">
         <v>8</v>
@@ -5191,7 +5206,7 @@
         <v>7</v>
       </c>
       <c r="O5" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P5" s="15" t="s">
         <v>8</v>
@@ -5206,7 +5221,7 @@
         <v>7</v>
       </c>
       <c r="T5" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U5" s="15" t="s">
         <v>8</v>
@@ -5221,7 +5236,7 @@
         <v>7</v>
       </c>
       <c r="Y5" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Z5" s="15" t="s">
         <v>8</v>
@@ -5236,7 +5251,7 @@
         <v>7</v>
       </c>
       <c r="AD5" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AE5" s="15" t="s">
         <v>8</v>
@@ -5268,7 +5283,7 @@
       <c r="H6" s="62">
         <v>28439.88</v>
       </c>
-      <c r="I6" s="82">
+      <c r="I6" s="75">
         <v>4.0888118807699998E-3</v>
       </c>
       <c r="J6" s="63">
@@ -5300,7 +5315,7 @@
       <c r="R6" s="62">
         <v>6475.72</v>
       </c>
-      <c r="S6" s="82">
+      <c r="S6" s="75">
         <v>0.66141675514800002</v>
       </c>
       <c r="T6" s="63">
@@ -5331,7 +5346,7 @@
       <c r="AB6" s="62">
         <v>43416.4</v>
       </c>
-      <c r="AC6" s="82">
+      <c r="AC6" s="75">
         <v>1.01703200463237E-2</v>
       </c>
       <c r="AD6" s="63">
@@ -5367,7 +5382,7 @@
       <c r="H7" s="66">
         <v>50689.52</v>
       </c>
-      <c r="I7" s="83">
+      <c r="I7" s="76">
         <v>4.3877273659700001E-4</v>
       </c>
       <c r="J7" s="67">
@@ -5399,7 +5414,7 @@
       <c r="R7" s="66">
         <v>1329.32</v>
       </c>
-      <c r="S7" s="83">
+      <c r="S7" s="76">
         <v>0.34610360097600001</v>
       </c>
       <c r="T7" s="67">
@@ -5431,7 +5446,7 @@
       <c r="AB7" s="66">
         <v>14335.04</v>
       </c>
-      <c r="AC7" s="83">
+      <c r="AC7" s="76">
         <v>1.5778135649961202E-2</v>
       </c>
       <c r="AD7" s="67">
@@ -5445,23 +5460,23 @@
     <row r="8" spans="1:31">
       <c r="F8" s="14"/>
       <c r="G8" s="2">
-        <f>G6-B6</f>
+        <f t="shared" ref="G8:J9" si="0">G6-B6</f>
         <v>884.55999999999767</v>
       </c>
       <c r="H8" s="2">
-        <f>H6-C6</f>
+        <f t="shared" si="0"/>
         <v>879.76000000000204</v>
       </c>
       <c r="I8" s="2">
-        <f>I6-D6</f>
+        <f t="shared" si="0"/>
         <v>-1.9463036969999924E-5</v>
       </c>
       <c r="J8" s="60">
-        <f>J6-E6</f>
+        <f t="shared" si="0"/>
         <v>2.4653199770000072</v>
       </c>
       <c r="K8" s="14">
-        <f t="shared" ref="K8" si="0">K6-F6</f>
+        <f t="shared" ref="K8" si="1">K6-F6</f>
         <v>7.8190762180000428E-3</v>
       </c>
       <c r="L8" s="4"/>
@@ -5502,23 +5517,23 @@
     <row r="9" spans="1:31">
       <c r="F9" s="14"/>
       <c r="G9" s="2">
-        <f>G7-B7</f>
+        <f t="shared" si="0"/>
         <v>33540.28</v>
       </c>
       <c r="H9" s="2">
-        <f>H7-C7</f>
+        <f t="shared" si="0"/>
         <v>22394.639999999996</v>
       </c>
       <c r="I9" s="2">
-        <f>I7-D7</f>
+        <f t="shared" si="0"/>
         <v>-2.0837649825400004E-4</v>
       </c>
       <c r="J9" s="60">
-        <f>J7-E7</f>
+        <f t="shared" si="0"/>
         <v>4.205720052700002</v>
       </c>
       <c r="K9" s="14">
-        <f t="shared" ref="K9" si="1">K7-F7</f>
+        <f t="shared" ref="K9" si="2">K7-F7</f>
         <v>2.7353336135000017E-2</v>
       </c>
       <c r="L9" s="4"/>
@@ -5560,7 +5575,7 @@
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="80"/>
+      <c r="D10" s="74"/>
       <c r="F10" s="14"/>
       <c r="L10" t="s">
         <v>23</v>
@@ -5576,48 +5591,48 @@
       <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:31">
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="77"/>
-      <c r="D12" s="81"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="76" t="s">
+      <c r="C12" s="81"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="77"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="77"/>
-      <c r="K12" s="78"/>
-      <c r="L12" s="76" t="s">
+      <c r="H12" s="81"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="M12" s="77"/>
-      <c r="N12" s="81"/>
-      <c r="O12" s="77"/>
-      <c r="P12" s="78"/>
-      <c r="Q12" s="76" t="s">
+      <c r="M12" s="81"/>
+      <c r="N12" s="83"/>
+      <c r="O12" s="81"/>
+      <c r="P12" s="82"/>
+      <c r="Q12" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="R12" s="77"/>
-      <c r="S12" s="81"/>
-      <c r="T12" s="77"/>
-      <c r="U12" s="78"/>
-      <c r="V12" s="76" t="s">
+      <c r="R12" s="81"/>
+      <c r="S12" s="83"/>
+      <c r="T12" s="81"/>
+      <c r="U12" s="82"/>
+      <c r="V12" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="W12" s="77"/>
-      <c r="X12" s="81"/>
-      <c r="Y12" s="77"/>
-      <c r="Z12" s="78"/>
-      <c r="AA12" s="76" t="s">
+      <c r="W12" s="81"/>
+      <c r="X12" s="83"/>
+      <c r="Y12" s="81"/>
+      <c r="Z12" s="82"/>
+      <c r="AA12" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="AB12" s="77"/>
-      <c r="AC12" s="81"/>
-      <c r="AD12" s="77"/>
-      <c r="AE12" s="78"/>
+      <c r="AB12" s="81"/>
+      <c r="AC12" s="83"/>
+      <c r="AD12" s="81"/>
+      <c r="AE12" s="82"/>
     </row>
     <row r="13" spans="1:31">
       <c r="A13" s="33" t="s">
@@ -5633,7 +5648,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F13" s="15" t="s">
         <v>8</v>
@@ -5648,7 +5663,7 @@
         <v>7</v>
       </c>
       <c r="J13" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K13" s="15" t="s">
         <v>8</v>
@@ -5663,7 +5678,7 @@
         <v>7</v>
       </c>
       <c r="O13" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P13" s="15" t="s">
         <v>8</v>
@@ -5678,7 +5693,7 @@
         <v>7</v>
       </c>
       <c r="T13" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U13" s="15" t="s">
         <v>8</v>
@@ -5693,7 +5708,7 @@
         <v>7</v>
       </c>
       <c r="Y13" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Z13" s="15" t="s">
         <v>8</v>
@@ -5708,7 +5723,7 @@
         <v>7</v>
       </c>
       <c r="AD13" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AE13" s="15" t="s">
         <v>8</v>
@@ -5740,7 +5755,7 @@
       <c r="H14" s="62">
         <v>20461.84</v>
       </c>
-      <c r="I14" s="82">
+      <c r="I14" s="75">
         <v>9.9580910894967803E-3</v>
       </c>
       <c r="J14" s="63">
@@ -5771,7 +5786,7 @@
       <c r="R14" s="62">
         <v>2054.84</v>
       </c>
-      <c r="S14" s="82">
+      <c r="S14" s="75">
         <v>0.15315927474300001</v>
       </c>
       <c r="T14" s="63">
@@ -5803,7 +5818,7 @@
       <c r="AB14" s="62">
         <v>38239.96</v>
       </c>
-      <c r="AC14" s="82">
+      <c r="AC14" s="75">
         <v>9.9580910894967803E-3</v>
       </c>
       <c r="AD14" s="63">
@@ -5840,7 +5855,7 @@
       <c r="H15" s="66">
         <v>161164.96</v>
       </c>
-      <c r="I15" s="83">
+      <c r="I15" s="76">
         <v>2.7762807068600001E-3</v>
       </c>
       <c r="J15" s="67">
@@ -5872,7 +5887,7 @@
       <c r="R15" s="66">
         <v>6724.76</v>
       </c>
-      <c r="S15" s="83">
+      <c r="S15" s="76">
         <v>0.253251056463</v>
       </c>
       <c r="T15" s="67">
@@ -5904,7 +5919,7 @@
       <c r="AB15" s="66">
         <v>43623.72</v>
       </c>
-      <c r="AC15" s="83">
+      <c r="AC15" s="76">
         <v>1.1335646942011101E-2</v>
       </c>
       <c r="AD15" s="67">
@@ -5921,12 +5936,12 @@
         <f>G14-B14</f>
         <v>78.07999999999447</v>
       </c>
-      <c r="H16" s="84">
+      <c r="H16" s="2">
         <f>H14-C14</f>
         <v>598.88000000000102</v>
       </c>
-      <c r="I16" s="84">
-        <f t="shared" ref="I16:I17" si="2">I14-D14</f>
+      <c r="I16" s="2">
+        <f t="shared" ref="I16:I17" si="3">I14-D14</f>
         <v>-1.2140370542391976E-4</v>
       </c>
       <c r="J16" s="60">
@@ -5978,12 +5993,12 @@
         <f>G15-B15</f>
         <v>-1271.8800000000047</v>
       </c>
-      <c r="H17" s="84">
+      <c r="H17" s="2">
         <f>H15-C15</f>
         <v>1605.7599999999802</v>
       </c>
-      <c r="I17" s="84">
-        <f t="shared" si="2"/>
+      <c r="I17" s="2">
+        <f t="shared" si="3"/>
         <v>-4.7284769169999696E-5</v>
       </c>
       <c r="J17" s="60">
@@ -6033,7 +6048,7 @@
       <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="80"/>
+      <c r="D18" s="74"/>
       <c r="F18" s="14"/>
       <c r="L18" t="s">
         <v>24</v>
@@ -6049,48 +6064,48 @@
       <c r="M19" s="4"/>
     </row>
     <row r="20" spans="1:31">
-      <c r="B20" s="76" t="s">
+      <c r="B20" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="77"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="78"/>
-      <c r="G20" s="76" t="s">
+      <c r="C20" s="81"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="77"/>
-      <c r="I20" s="81"/>
-      <c r="J20" s="77"/>
-      <c r="K20" s="78"/>
-      <c r="L20" s="76" t="s">
+      <c r="H20" s="81"/>
+      <c r="I20" s="83"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="82"/>
+      <c r="L20" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="M20" s="77"/>
-      <c r="N20" s="81"/>
-      <c r="O20" s="77"/>
-      <c r="P20" s="78"/>
-      <c r="Q20" s="76" t="s">
+      <c r="M20" s="81"/>
+      <c r="N20" s="83"/>
+      <c r="O20" s="81"/>
+      <c r="P20" s="82"/>
+      <c r="Q20" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="R20" s="77"/>
-      <c r="S20" s="81"/>
-      <c r="T20" s="77"/>
-      <c r="U20" s="78"/>
-      <c r="V20" s="76" t="s">
+      <c r="R20" s="81"/>
+      <c r="S20" s="83"/>
+      <c r="T20" s="81"/>
+      <c r="U20" s="82"/>
+      <c r="V20" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="W20" s="77"/>
-      <c r="X20" s="81"/>
-      <c r="Y20" s="77"/>
-      <c r="Z20" s="78"/>
-      <c r="AA20" s="76" t="s">
+      <c r="W20" s="81"/>
+      <c r="X20" s="83"/>
+      <c r="Y20" s="81"/>
+      <c r="Z20" s="82"/>
+      <c r="AA20" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="AB20" s="77"/>
-      <c r="AC20" s="81"/>
-      <c r="AD20" s="77"/>
-      <c r="AE20" s="78"/>
+      <c r="AB20" s="81"/>
+      <c r="AC20" s="83"/>
+      <c r="AD20" s="81"/>
+      <c r="AE20" s="82"/>
     </row>
     <row r="21" spans="1:31">
       <c r="A21" s="33" t="s">
@@ -6106,7 +6121,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>8</v>
@@ -6121,7 +6136,7 @@
         <v>7</v>
       </c>
       <c r="J21" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K21" s="15" t="s">
         <v>8</v>
@@ -6136,7 +6151,7 @@
         <v>7</v>
       </c>
       <c r="O21" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P21" s="15" t="s">
         <v>8</v>
@@ -6151,7 +6166,7 @@
         <v>7</v>
       </c>
       <c r="T21" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U21" s="15" t="s">
         <v>8</v>
@@ -6166,7 +6181,7 @@
         <v>7</v>
       </c>
       <c r="Y21" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Z21" s="15" t="s">
         <v>8</v>
@@ -6181,7 +6196,7 @@
         <v>7</v>
       </c>
       <c r="AD21" s="60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AE21" s="15" t="s">
         <v>8</v>
@@ -6213,7 +6228,7 @@
       <c r="H22" s="62">
         <v>1850.8</v>
       </c>
-      <c r="I22" s="82">
+      <c r="I22" s="75">
         <v>1.3221012618700001E-3</v>
       </c>
       <c r="J22" s="63">
@@ -6245,7 +6260,7 @@
       <c r="R22" s="62">
         <v>394.84</v>
       </c>
-      <c r="S22" s="82">
+      <c r="S22" s="75">
         <v>3.05458604952944E-2</v>
       </c>
       <c r="T22" s="63">
@@ -6277,7 +6292,7 @@
       <c r="AB22" s="62">
         <v>48301.440000000002</v>
       </c>
-      <c r="AC22" s="82">
+      <c r="AC22" s="75">
         <v>9.3614011579710597E-4</v>
       </c>
       <c r="AD22" s="63">
@@ -6314,7 +6329,7 @@
       <c r="H23" s="66">
         <v>42978.879999999997</v>
       </c>
-      <c r="I23" s="83">
+      <c r="I23" s="76">
         <v>3.3760500982900002E-4</v>
       </c>
       <c r="J23" s="67">
@@ -6346,7 +6361,7 @@
       <c r="R23" s="66">
         <v>8438.16</v>
       </c>
-      <c r="S23" s="83">
+      <c r="S23" s="76">
         <v>5.2383032633299999E-2</v>
       </c>
       <c r="T23" s="67">
@@ -6378,7 +6393,7 @@
       <c r="AB23" s="66">
         <v>47900.56</v>
       </c>
-      <c r="AC23" s="83">
+      <c r="AC23" s="76">
         <v>6.1632317997577203E-4</v>
       </c>
       <c r="AD23" s="67">
@@ -6399,7 +6414,7 @@
         <v>596.52</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" ref="I24:I25" si="3">I22-D22</f>
+        <f t="shared" ref="I24:I25" si="4">I22-D22</f>
         <v>-4.94193417799999E-5</v>
       </c>
       <c r="J24" s="60">
@@ -6453,7 +6468,7 @@
         <v>245.87999999999738</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-3.6619887469999828E-6</v>
       </c>
       <c r="J25" s="60">
@@ -6493,17 +6508,18 @@
         <v>-2.9824757575989018</v>
       </c>
       <c r="AE25" s="70">
-        <f t="shared" ref="AE25" si="4">AE23-Z23</f>
+        <f t="shared" ref="AE25" si="5">AE23-Z23</f>
         <v>3.707276530913961E-3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="L20:P20"/>
-    <mergeCell ref="Q20:U20"/>
-    <mergeCell ref="V20:Z20"/>
+    <mergeCell ref="AA4:AE4"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="V4:Z4"/>
     <mergeCell ref="AA20:AE20"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="G12:K12"/>
@@ -6511,12 +6527,11 @@
     <mergeCell ref="Q12:U12"/>
     <mergeCell ref="V12:Z12"/>
     <mergeCell ref="AA12:AE12"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="L4:P4"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="V4:Z4"/>
-    <mergeCell ref="AA4:AE4"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="L20:P20"/>
+    <mergeCell ref="Q20:U20"/>
+    <mergeCell ref="V20:Z20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7554,10 +7569,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95DB78E-C3C9-4D84-AB69-47409FDD14D6}">
-  <dimension ref="B3:G42"/>
+  <dimension ref="B3:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H26" sqref="B24:I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7566,8 +7581,10 @@
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7">
@@ -7645,7 +7662,7 @@
       <c r="E6">
         <v>-23.426223312313699</v>
       </c>
-      <c r="F6" s="79">
+      <c r="F6" s="73">
         <v>4.8137919979846798E-18</v>
       </c>
       <c r="G6" t="b">
@@ -7666,7 +7683,7 @@
       <c r="E7">
         <v>-14.297332990836001</v>
       </c>
-      <c r="F7" s="79">
+      <c r="F7" s="73">
         <v>3.0714612725714102E-13</v>
       </c>
       <c r="G7" t="b">
@@ -7729,7 +7746,7 @@
       <c r="E10">
         <v>-12.112149888197999</v>
       </c>
-      <c r="F10" s="79">
+      <c r="F10" s="73">
         <v>1.03067926866572E-11</v>
       </c>
       <c r="G10" t="b">
@@ -7813,7 +7830,7 @@
       <c r="E14">
         <v>-6.8462529407336197</v>
       </c>
-      <c r="F14" s="79">
+      <c r="F14" s="73">
         <v>4.4238056566889001E-7</v>
       </c>
       <c r="G14" t="b">
@@ -7855,7 +7872,7 @@
       <c r="E16">
         <v>-30.993361936174601</v>
       </c>
-      <c r="F16" s="79">
+      <c r="F16" s="73">
         <v>7.1735146545689301E-21</v>
       </c>
       <c r="G16" t="b">
@@ -7863,7 +7880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:9">
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -7884,7 +7901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:9">
       <c r="B18" t="s">
         <v>18</v>
       </c>
@@ -7897,7 +7914,7 @@
       <c r="E18">
         <v>-23.426223312313699</v>
       </c>
-      <c r="F18" s="79">
+      <c r="F18" s="73">
         <v>4.8137919979846798E-18</v>
       </c>
       <c r="G18" t="b">
@@ -7905,7 +7922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:9">
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -7926,7 +7943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:9">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -7947,7 +7964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:9">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -7960,7 +7977,7 @@
       <c r="E21">
         <v>-96.983270019834706</v>
       </c>
-      <c r="F21" s="79">
+      <c r="F21" s="73">
         <v>1.1922100634926601E-32</v>
       </c>
       <c r="G21" t="b">
@@ -7968,7 +7985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:9">
       <c r="B24" t="s">
         <v>66</v>
       </c>
@@ -7979,13 +7996,22 @@
         <v>20</v>
       </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7">
+        <v>73</v>
+      </c>
+      <c r="G24" t="s">
+        <v>75</v>
+      </c>
+      <c r="H24" t="s">
+        <v>74</v>
+      </c>
+      <c r="I24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
       <c r="B25" t="s">
         <v>4</v>
       </c>
@@ -7998,12 +8024,22 @@
       <c r="E25">
         <v>0.25372924677457598</v>
       </c>
-      <c r="F25" s="1" t="str">
-        <f>IF(E25&lt;0.05, "Yes", "No")</f>
+      <c r="F25">
+        <v>0.572209586790842</v>
+      </c>
+      <c r="G25" s="1" t="str">
+        <f t="shared" ref="G25:G42" si="1">IF(E25&lt;0.05, "Yes", "No")</f>
         <v>No</v>
       </c>
-    </row>
-    <row r="26" spans="2:7">
+      <c r="H25" s="1" t="str">
+        <f t="shared" ref="H25:H42" si="2">IF(F25&lt;0.05, "Yes", "No")</f>
+        <v>No</v>
+      </c>
+      <c r="I25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -8016,12 +8052,22 @@
       <c r="E26">
         <v>0.75341035855965799</v>
       </c>
-      <c r="F26" s="1" t="str">
-        <f t="shared" ref="F26:F42" si="1">IF(E26&lt;0.05, "Yes", "No")</f>
+      <c r="F26" s="73">
+        <v>2.07973885106272E-9</v>
+      </c>
+      <c r="G26" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="27" spans="2:7">
+      <c r="H26" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="I26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9">
       <c r="B27" t="s">
         <v>4</v>
       </c>
@@ -8031,15 +8077,25 @@
       <c r="D27" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="79">
+      <c r="E27" s="73">
         <v>4.8137919979846798E-18</v>
       </c>
-      <c r="F27" t="str">
+      <c r="F27" s="73">
+        <v>2.4419157037155599E-5</v>
+      </c>
+      <c r="G27" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="28" spans="2:7">
+      <c r="H27" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="I27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
       <c r="B28" t="s">
         <v>4</v>
       </c>
@@ -8049,15 +8105,25 @@
       <c r="D28" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="79">
+      <c r="E28" s="73">
         <v>3.0714612725714102E-13</v>
       </c>
-      <c r="F28" t="str">
+      <c r="F28" s="73">
+        <v>1.1707636440496301E-5</v>
+      </c>
+      <c r="G28" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="29" spans="2:7">
+      <c r="H28" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="I28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
       <c r="B29" t="s">
         <v>4</v>
       </c>
@@ -8070,12 +8136,22 @@
       <c r="E29">
         <v>0.68271670620649105</v>
       </c>
-      <c r="F29" s="1" t="str">
+      <c r="F29">
+        <v>0.86723836461891901</v>
+      </c>
+      <c r="G29" s="1" t="str">
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="30" spans="2:7">
+      <c r="H29" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="I29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
       <c r="B30" t="s">
         <v>4</v>
       </c>
@@ -8088,12 +8164,22 @@
       <c r="E30">
         <v>4.2880921906591899E-4</v>
       </c>
-      <c r="F30" t="str">
+      <c r="F30">
+        <v>0.65627091705812801</v>
+      </c>
+      <c r="G30" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="31" spans="2:7">
+      <c r="H30" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="I30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9">
       <c r="B31" t="s">
         <v>14</v>
       </c>
@@ -8103,15 +8189,25 @@
       <c r="D31" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="79">
+      <c r="E31" s="73">
         <v>1.03067926866572E-11</v>
       </c>
-      <c r="F31" t="str">
+      <c r="F31" s="73">
+        <v>1.02054324171284E-21</v>
+      </c>
+      <c r="G31" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="32" spans="2:7">
+      <c r="H31" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="I31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9">
       <c r="B32" t="s">
         <v>14</v>
       </c>
@@ -8124,12 +8220,22 @@
       <c r="E32">
         <v>0.64887258439009499</v>
       </c>
-      <c r="F32" s="1" t="str">
+      <c r="F32">
+        <v>0.165678432033633</v>
+      </c>
+      <c r="G32" s="1" t="str">
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="33" spans="2:6">
+      <c r="H32" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="I32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9">
       <c r="B33" t="s">
         <v>14</v>
       </c>
@@ -8142,12 +8248,22 @@
       <c r="E33">
         <v>0.29951326413134899</v>
       </c>
-      <c r="F33" s="1" t="str">
+      <c r="F33">
+        <v>1.7188758797908502E-2</v>
+      </c>
+      <c r="G33" s="1" t="str">
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="34" spans="2:6">
+      <c r="H33" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="I33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9">
       <c r="B34" t="s">
         <v>14</v>
       </c>
@@ -8160,12 +8276,22 @@
       <c r="E34">
         <v>7.3993424288121296E-3</v>
       </c>
-      <c r="F34" t="str">
+      <c r="F34" s="73">
+        <v>1.2876378866076E-19</v>
+      </c>
+      <c r="G34" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="35" spans="2:6">
+      <c r="H34" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="I34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9">
       <c r="B35" t="s">
         <v>14</v>
       </c>
@@ -8175,15 +8301,25 @@
       <c r="D35" t="s">
         <v>27</v>
       </c>
-      <c r="E35" s="79">
+      <c r="E35" s="73">
         <v>4.4238056566889001E-7</v>
       </c>
-      <c r="F35" t="str">
+      <c r="F35" s="73">
+        <v>7.3733241807256095E-18</v>
+      </c>
+      <c r="G35" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="36" spans="2:6">
+      <c r="H35" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="I35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9">
       <c r="B36" t="s">
         <v>14</v>
       </c>
@@ -8196,12 +8332,22 @@
       <c r="E36">
         <v>0.48526860203996602</v>
       </c>
-      <c r="F36" s="1" t="str">
+      <c r="F36">
+        <v>4.8997988349383504E-4</v>
+      </c>
+      <c r="G36" s="1" t="str">
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="37" spans="2:6">
+      <c r="H36" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="I36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9">
       <c r="B37" t="s">
         <v>18</v>
       </c>
@@ -8211,15 +8357,25 @@
       <c r="D37" t="s">
         <v>53</v>
       </c>
-      <c r="E37" s="79">
+      <c r="E37" s="73">
         <v>7.1735146545689301E-21</v>
       </c>
-      <c r="F37" t="str">
+      <c r="F37">
+        <v>0.12796602261280299</v>
+      </c>
+      <c r="G37" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="38" spans="2:6">
+      <c r="H37" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="I37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9">
       <c r="B38" t="s">
         <v>18</v>
       </c>
@@ -8232,12 +8388,22 @@
       <c r="E38">
         <v>0.67158672847322398</v>
       </c>
-      <c r="F38" s="1" t="str">
+      <c r="F38">
+        <v>4.1895820194385702E-2</v>
+      </c>
+      <c r="G38" s="1" t="str">
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="39" spans="2:6">
+      <c r="H38" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="I38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9">
       <c r="B39" t="s">
         <v>18</v>
       </c>
@@ -8247,15 +8413,25 @@
       <c r="D39" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="79">
+      <c r="E39" s="73">
         <v>4.8137919979846798E-18</v>
       </c>
-      <c r="F39" t="str">
+      <c r="F39" s="73">
+        <v>2.4419157037155599E-5</v>
+      </c>
+      <c r="G39" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="40" spans="2:6">
+      <c r="H39" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="I39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
       <c r="B40" t="s">
         <v>18</v>
       </c>
@@ -8268,12 +8444,22 @@
       <c r="E40">
         <v>0.72972028676733203</v>
       </c>
-      <c r="F40" s="1" t="str">
+      <c r="F40">
+        <v>6.0443441667539198E-2</v>
+      </c>
+      <c r="G40" s="1" t="str">
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="41" spans="2:6">
+      <c r="H40" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="I40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9">
       <c r="B41" t="s">
         <v>18</v>
       </c>
@@ -8286,12 +8472,22 @@
       <c r="E41">
         <v>3.5952710792857202E-2</v>
       </c>
-      <c r="F41" t="str">
+      <c r="F41" s="73">
+        <v>1.2921747133469399E-5</v>
+      </c>
+      <c r="G41" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="42" spans="2:6">
+      <c r="H41" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+      <c r="I41" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9">
       <c r="B42" t="s">
         <v>18</v>
       </c>
@@ -8301,12 +8497,22 @@
       <c r="D42" t="s">
         <v>27</v>
       </c>
-      <c r="E42" s="79">
+      <c r="E42" s="73">
         <v>1.1922100634926601E-32</v>
       </c>
-      <c r="F42" t="str">
+      <c r="F42">
+        <v>0.84227227894214896</v>
+      </c>
+      <c r="G42" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
+      </c>
+      <c r="H42" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+      <c r="I42" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added results and bump charts updated
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Monash_University\Year5\Honours_Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7897E318-15D4-46F1-BF46-D6CA28AA1C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881F25D9-2B3C-4827-A527-A38D409678EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{52DF0958-0AB4-4740-8193-FA00E6A62DB5}"/>
+    <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{52DF0958-0AB4-4740-8193-FA00E6A62DB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Old" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,9 @@
     <sheet name="latest_data" sheetId="10" r:id="rId5"/>
     <sheet name="correlation_coefficients" sheetId="8" r:id="rId6"/>
     <sheet name="t-test" sheetId="9" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="83">
   <si>
     <t>TSN = Total number of generated samples</t>
   </si>
@@ -281,6 +281,18 @@
   <si>
     <t>Combined Results</t>
   </si>
+  <si>
+    <t>DT - MLPC</t>
+  </si>
+  <si>
+    <t>MLPC - RF</t>
+  </si>
+  <si>
+    <t>DT - RF</t>
+  </si>
+  <si>
+    <t>Bank Marketing</t>
+  </si>
 </sst>
 </file>
 
@@ -476,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -575,6 +587,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2507,6 +2522,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="S12:V12"/>
+    <mergeCell ref="W12:Z12"/>
+    <mergeCell ref="S20:V20"/>
+    <mergeCell ref="W20:Z20"/>
     <mergeCell ref="C20:F20"/>
     <mergeCell ref="G20:J20"/>
     <mergeCell ref="K20:N20"/>
@@ -2520,11 +2540,6 @@
     <mergeCell ref="G12:J12"/>
     <mergeCell ref="K12:N12"/>
     <mergeCell ref="O12:R12"/>
-    <mergeCell ref="W4:Z4"/>
-    <mergeCell ref="S12:V12"/>
-    <mergeCell ref="W12:Z12"/>
-    <mergeCell ref="S20:V20"/>
-    <mergeCell ref="W20:Z20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3778,6 +3793,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:U4"/>
     <mergeCell ref="V20:Y20"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="F12:I12"/>
@@ -3790,12 +3811,6 @@
     <mergeCell ref="J20:M20"/>
     <mergeCell ref="N20:Q20"/>
     <mergeCell ref="R20:U20"/>
-    <mergeCell ref="V4:Y4"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:U4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5042,12 +5057,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="V4:Y4"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:U4"/>
     <mergeCell ref="V20:Y20"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="F12:I12"/>
@@ -5060,6 +5069,12 @@
     <mergeCell ref="J20:M20"/>
     <mergeCell ref="N20:Q20"/>
     <mergeCell ref="R20:U20"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:U4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5071,7 +5086,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V10" sqref="V10"/>
+      <selection pane="topRight" activeCell="AC23" sqref="AC23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5158,7 +5173,7 @@
         <v>19</v>
       </c>
       <c r="AB4" s="81"/>
-      <c r="AC4" s="83"/>
+      <c r="AC4" s="84"/>
       <c r="AD4" s="81"/>
       <c r="AE4" s="82"/>
     </row>
@@ -5467,7 +5482,7 @@
         <f t="shared" si="0"/>
         <v>879.76000000000204</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="3">
         <f t="shared" si="0"/>
         <v>-1.9463036969999924E-5</v>
       </c>
@@ -5489,6 +5504,10 @@
         <f>R6-M6</f>
         <v>1418.8400000000001</v>
       </c>
+      <c r="S8" s="3">
+        <f t="shared" ref="S8:S9" si="2">S6-N6</f>
+        <v>0.44352547029900002</v>
+      </c>
       <c r="T8" s="60">
         <f>T6-O6</f>
         <v>1.8097199535399993</v>
@@ -5504,6 +5523,10 @@
       <c r="AB8" s="2">
         <f>AB6-W6</f>
         <v>1275.0800000000017</v>
+      </c>
+      <c r="AC8" s="3">
+        <f t="shared" ref="AC8:AC9" si="3">AC6-X6</f>
+        <v>-2.7572852442589967E-4</v>
       </c>
       <c r="AD8" s="60">
         <f>AD6-Y6</f>
@@ -5524,7 +5547,7 @@
         <f t="shared" si="0"/>
         <v>22394.639999999996</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="3">
         <f t="shared" si="0"/>
         <v>-2.0837649825400004E-4</v>
       </c>
@@ -5533,7 +5556,7 @@
         <v>4.205720052700002</v>
       </c>
       <c r="K9" s="14">
-        <f t="shared" ref="K9" si="2">K7-F7</f>
+        <f t="shared" ref="K9" si="4">K7-F7</f>
         <v>2.7353336135000017E-2</v>
       </c>
       <c r="L9" s="4"/>
@@ -5546,6 +5569,10 @@
         <f>R7-M7</f>
         <v>-201.48000000000002</v>
       </c>
+      <c r="S9" s="3">
+        <f t="shared" si="2"/>
+        <v>0.26182871863069612</v>
+      </c>
       <c r="T9" s="71">
         <f>T7-O7</f>
         <v>328.667519932</v>
@@ -5561,6 +5588,10 @@
       <c r="AB9" s="2">
         <f>AB7-W7</f>
         <v>-468.47999999999956</v>
+      </c>
+      <c r="AC9" s="3">
+        <f t="shared" si="3"/>
+        <v>2.069875667670501E-3</v>
       </c>
       <c r="AD9" s="71">
         <f>AD7-Y7</f>
@@ -5630,7 +5661,7 @@
         <v>19</v>
       </c>
       <c r="AB12" s="81"/>
-      <c r="AC12" s="83"/>
+      <c r="AC12" s="84"/>
       <c r="AD12" s="81"/>
       <c r="AE12" s="82"/>
     </row>
@@ -5940,8 +5971,8 @@
         <f>H14-C14</f>
         <v>598.88000000000102</v>
       </c>
-      <c r="I16" s="2">
-        <f t="shared" ref="I16:I17" si="3">I14-D14</f>
+      <c r="I16" s="3">
+        <f t="shared" ref="I16:I17" si="5">I14-D14</f>
         <v>-1.2140370542391976E-4</v>
       </c>
       <c r="J16" s="60">
@@ -5962,6 +5993,10 @@
         <f>R14-M14</f>
         <v>99.360000000000127</v>
       </c>
+      <c r="S16" s="3">
+        <f t="shared" ref="S16:S17" si="6">S14-N14</f>
+        <v>1.0385825289000006E-2</v>
+      </c>
       <c r="T16" s="60">
         <f>T14-O14</f>
         <v>33.887359971999956</v>
@@ -5977,6 +6012,10 @@
       <c r="AB16" s="2">
         <f>AB14-W14</f>
         <v>-12669</v>
+      </c>
+      <c r="AC16" s="3">
+        <f t="shared" ref="AC16:AC17" si="7">AC14-X14</f>
+        <v>-1.2140370542391976E-4</v>
       </c>
       <c r="AD16" s="60">
         <f>AD14-Y14</f>
@@ -5997,8 +6036,8 @@
         <f>H15-C15</f>
         <v>1605.7599999999802</v>
       </c>
-      <c r="I17" s="2">
-        <f t="shared" si="3"/>
+      <c r="I17" s="3">
+        <f t="shared" si="5"/>
         <v>-4.7284769169999696E-5</v>
       </c>
       <c r="J17" s="60">
@@ -6019,6 +6058,10 @@
         <f>R15-M15</f>
         <v>-109.31999999999971</v>
       </c>
+      <c r="S17" s="3">
+        <f t="shared" si="6"/>
+        <v>-1.4920097906000018E-2</v>
+      </c>
       <c r="T17" s="71">
         <f>T15-O15</f>
         <v>-101.88599997000006</v>
@@ -6034,6 +6077,10 @@
       <c r="AB17" s="2">
         <f>AB15-W15</f>
         <v>405.31999999999971</v>
+      </c>
+      <c r="AC17" s="3">
+        <f t="shared" si="7"/>
+        <v>2.8169890518497404E-3</v>
       </c>
       <c r="AD17" s="60">
         <f>AD15-Y15</f>
@@ -6103,7 +6150,7 @@
         <v>19</v>
       </c>
       <c r="AB20" s="81"/>
-      <c r="AC20" s="83"/>
+      <c r="AC20" s="84"/>
       <c r="AD20" s="81"/>
       <c r="AE20" s="82"/>
     </row>
@@ -6244,7 +6291,7 @@
       <c r="M22" s="4">
         <v>383.36</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="3">
         <v>1.8658029371758499E-2</v>
       </c>
       <c r="O22" s="60">
@@ -6413,8 +6460,8 @@
         <f>H22-C22</f>
         <v>596.52</v>
       </c>
-      <c r="I24" s="2">
-        <f t="shared" ref="I24:I25" si="4">I22-D22</f>
+      <c r="I24" s="3">
+        <f t="shared" ref="I24:I25" si="8">I22-D22</f>
         <v>-4.94193417799999E-5</v>
       </c>
       <c r="J24" s="60">
@@ -6433,6 +6480,10 @@
         <f>R22-M22</f>
         <v>11.479999999999961</v>
       </c>
+      <c r="S24" s="3">
+        <f t="shared" ref="S24:S25" si="9">S22-N22</f>
+        <v>1.1887831123535902E-2</v>
+      </c>
       <c r="T24" s="60">
         <f>T22-O22</f>
         <v>1.8097199535399993</v>
@@ -6448,6 +6499,10 @@
       <c r="AB24" s="2">
         <f>AB22-W22</f>
         <v>-1978</v>
+      </c>
+      <c r="AC24" s="3">
+        <f t="shared" ref="AC24:AC25" si="10">AC22-X22</f>
+        <v>2.6142909984512921E-5</v>
       </c>
       <c r="AD24" s="60">
         <f>AD22-Y22</f>
@@ -6467,8 +6522,8 @@
         <f>H23-C23</f>
         <v>245.87999999999738</v>
       </c>
-      <c r="I25" s="2">
-        <f t="shared" si="4"/>
+      <c r="I25" s="3">
+        <f t="shared" si="8"/>
         <v>-3.6619887469999828E-6</v>
       </c>
       <c r="J25" s="60">
@@ -6487,6 +6542,10 @@
         <f>R23-M23</f>
         <v>3352</v>
       </c>
+      <c r="S25" s="3">
+        <f t="shared" si="9"/>
+        <v>1.5050434143760998E-2</v>
+      </c>
       <c r="T25" s="71">
         <f>T23-O23</f>
         <v>228.849320068</v>
@@ -6503,23 +6562,21 @@
         <f>AB23-W23</f>
         <v>-2028.6399999999994</v>
       </c>
+      <c r="AC25" s="3">
+        <f t="shared" si="10"/>
+        <v>-3.4679351558272969E-5</v>
+      </c>
       <c r="AD25" s="60">
         <f>AD23-Y23</f>
         <v>-2.9824757575989018</v>
       </c>
       <c r="AE25" s="70">
-        <f t="shared" ref="AE25" si="5">AE23-Z23</f>
+        <f t="shared" ref="AE25" si="11">AE23-Z23</f>
         <v>3.707276530913961E-3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="AA4:AE4"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="L4:P4"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="V4:Z4"/>
     <mergeCell ref="AA20:AE20"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="G12:K12"/>
@@ -6532,6 +6589,12 @@
     <mergeCell ref="L20:P20"/>
     <mergeCell ref="Q20:U20"/>
     <mergeCell ref="V20:Z20"/>
+    <mergeCell ref="AA4:AE4"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="V4:Z4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7571,8 +7634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95DB78E-C3C9-4D84-AB69-47409FDD14D6}">
   <dimension ref="B3:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H26" sqref="B24:I42"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8518,4 +8581,67 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E71E7E2-BDE0-4081-9D6A-B6CF18B81DDD}">
+  <dimension ref="B2:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4">
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>